<commit_message>
Improved dep ttest and ui
</commit_message>
<xml_diff>
--- a/dataPublic/testObserverData.xlsx
+++ b/dataPublic/testObserverData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\ZlabCode\qtProjects\autograph_behavior\dataPublic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0199844D-AB0C-4A79-A0B7-B07D01FC5535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68FDC19-EA07-40D1-B7D9-8AE7C4E5DEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5310" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,18 +475,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.5546875" customWidth="1"/>
   </cols>

</xml_diff>